<commit_message>
Creazione Controllo del movimento
Cartella 0-3 anni fatto da Gio il 22/04/2020
</commit_message>
<xml_diff>
--- a/esplora.xlsx
+++ b/esplora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\iomimuovoacasa.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF10C85-E7D3-4BBF-984A-E37F38862560}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F31120F-7D1C-4A60-A3D0-E22C37CD3EBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A057EE54-A210-47BF-8DD6-CC519B554E7A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Cartella</t>
   </si>
@@ -198,7 +198,7 @@
     <t>Neuro e psicomotorio</t>
   </si>
   <si>
-    <t>Insieme di esercizi finalizzati al miglioramento del controllo del movimento.</t>
+    <t>Insieme di esercizi finalizzati al miglioramento del controllo della coordinazione motoria.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +655,15 @@
       <c r="L2" t="s">
         <v>24</v>
       </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Tentativo 2 immagine mobolizzazione
</commit_message>
<xml_diff>
--- a/esplora.xlsx
+++ b/esplora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\iomimuovoacasa.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F56A23-B763-479D-BD6F-9CEDAFE129B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A36AA-51F8-4614-A3E3-9DED7FA761E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A057EE54-A210-47BF-8DD6-CC519B554E7A}"/>
   </bookViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF098EE6-17AB-455A-AB98-AF8837D06DB4}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>